<commit_message>
use PyTK to package data analysis tools and build GUI
</commit_message>
<xml_diff>
--- a/EP05_result/20190830_EP05_result.xlsx
+++ b/EP05_result/20190830_EP05_result.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\ELISA\EP05_06_analysis_forCGU_toGitHub\EP05_result\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12143"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="C" sheetId="3" r:id="rId3"/>
     <sheet name="D" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="47">
   <si>
     <t>SS</t>
   </si>
@@ -155,17 +160,21 @@
   </si>
   <si>
     <t>9.4663 - 13.5001</t>
+  </si>
+  <si>
+    <t>nestANOVA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -173,8 +182,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -220,15 +236,92 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="新細明體"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表格1" displayName="表格1" ref="A1:K5" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="A1:K5"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="nestANOVA" dataDxfId="1"/>
+    <tableColumn id="2" name="SS"/>
+    <tableColumn id="3" name="MS"/>
+    <tableColumn id="4" name="df"/>
+    <tableColumn id="5" name="F"/>
+    <tableColumn id="6" name="p-value"/>
+    <tableColumn id="7" name="Variance"/>
+    <tableColumn id="8" name="SD"/>
+    <tableColumn id="9" name="CV%"/>
+    <tableColumn id="10" name="95%CI of SD"/>
+    <tableColumn id="11" name="95%CI of CV%"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -270,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,9 +395,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,6 +430,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,72 +606,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="32.2109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.35546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>9607117.616518497</v>
+        <v>9607117.6165184975</v>
       </c>
       <c r="C2">
-        <v>505637.7692904472</v>
+        <v>505637.76929044718</v>
       </c>
       <c r="D2">
         <v>19</v>
       </c>
       <c r="E2">
-        <v>4.857327986937304</v>
+        <v>4.8573279869373041</v>
       </c>
       <c r="F2">
-        <v>0.0004633279306719965</v>
+        <v>4.6332793067199648E-4</v>
       </c>
       <c r="G2">
         <v>100384.9608252615</v>
       </c>
       <c r="H2">
-        <v>316.8358578590206</v>
+        <v>316.83585785902062</v>
       </c>
       <c r="I2">
-        <v>7.233948407944784</v>
+        <v>7.2339484079447844</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
@@ -585,15 +691,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
         <v>2081958.519788027</v>
       </c>
       <c r="C3">
-        <v>104097.9259894013</v>
+        <v>104097.92598940129</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -602,16 +708,16 @@
         <v>2.479915203021589</v>
       </c>
       <c r="F3">
-        <v>0.007144591842550267</v>
+        <v>7.144591842550267E-3</v>
       </c>
       <c r="G3">
         <v>31060.76028063893</v>
       </c>
       <c r="H3">
-        <v>176.2406317528365</v>
+        <v>176.24063175283649</v>
       </c>
       <c r="I3">
-        <v>4.023899460429449</v>
+        <v>4.0238994604294493</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
@@ -620,27 +726,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4">
         <v>1679056.217124939</v>
       </c>
       <c r="C4">
-        <v>41976.40542812347</v>
+        <v>41976.405428123471</v>
       </c>
       <c r="D4">
         <v>40</v>
       </c>
       <c r="G4">
-        <v>41976.40542812347</v>
+        <v>41976.405428123471</v>
       </c>
       <c r="H4">
-        <v>204.8814423712491</v>
+        <v>204.88144237124911</v>
       </c>
       <c r="I4">
-        <v>4.677822118601251</v>
+        <v>4.6778221186012514</v>
       </c>
       <c r="J4" t="s">
         <v>16</v>
@@ -649,15 +755,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5">
         <v>13368132.35343146</v>
       </c>
       <c r="C5">
-        <v>169216.8652333097</v>
+        <v>169216.86523330971</v>
       </c>
       <c r="D5">
         <v>33.94899922662109</v>
@@ -669,7 +775,7 @@
         <v>416.4398234247343</v>
       </c>
       <c r="I5">
-        <v>9.508091091787371</v>
+        <v>9.5080910917873709</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -679,19 +785,23 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,33 +833,33 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>5204844.36818862</v>
+        <v>5204844.3681886196</v>
       </c>
       <c r="C2">
-        <v>273939.1772730852</v>
+        <v>273939.17727308522</v>
       </c>
       <c r="D2">
         <v>19</v>
       </c>
       <c r="E2">
-        <v>3.582151125726986</v>
+        <v>3.5821511257269858</v>
       </c>
       <c r="F2">
-        <v>0.003339398918661373</v>
+        <v>3.339398918661373E-3</v>
       </c>
       <c r="G2">
-        <v>49366.45120136204</v>
+        <v>49366.451201362041</v>
       </c>
       <c r="H2">
-        <v>222.1856233003433</v>
+        <v>222.18562330034331</v>
       </c>
       <c r="I2">
-        <v>7.022063788913891</v>
+        <v>7.0220637889138908</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
@@ -758,7 +868,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -766,25 +876,25 @@
         <v>1529467.449352741</v>
       </c>
       <c r="C3">
-        <v>76473.37246763706</v>
+        <v>76473.372467637062</v>
       </c>
       <c r="D3">
         <v>20</v>
       </c>
       <c r="E3">
-        <v>4.796454579842159</v>
+        <v>4.7964545798421589</v>
       </c>
       <c r="F3">
-        <v>1.247372195392716e-05</v>
+        <v>1.247372195392716E-5</v>
       </c>
       <c r="G3">
         <v>30264.82168317437</v>
       </c>
       <c r="H3">
-        <v>173.9678754344444</v>
+        <v>173.96787543444441</v>
       </c>
       <c r="I3">
-        <v>5.498166354675239</v>
+        <v>5.4981663546752388</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
@@ -793,12 +903,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>637749.1640515327</v>
+        <v>637749.16405153275</v>
       </c>
       <c r="C4">
         <v>15943.72910128832</v>
@@ -810,10 +920,10 @@
         <v>15943.72910128832</v>
       </c>
       <c r="H4">
-        <v>126.2684802367096</v>
+        <v>126.26848023670961</v>
       </c>
       <c r="I4">
-        <v>3.990651193271953</v>
+        <v>3.9906511932719528</v>
       </c>
       <c r="J4" t="s">
         <v>24</v>
@@ -822,27 +932,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5">
-        <v>7372060.981592894</v>
+        <v>7372060.9815928936</v>
       </c>
       <c r="C5">
-        <v>93317.22761509992</v>
+        <v>93317.227615099924</v>
       </c>
       <c r="D5">
-        <v>34.24844358499332</v>
+        <v>34.248443584993318</v>
       </c>
       <c r="G5">
-        <v>95575.00198582473</v>
+        <v>95575.001985824725</v>
       </c>
       <c r="H5">
-        <v>309.1520693539422</v>
+        <v>309.15206935394218</v>
       </c>
       <c r="I5">
-        <v>9.770594151105723</v>
+        <v>9.7705941511057226</v>
       </c>
       <c r="J5" t="s">
         <v>25</v>
@@ -852,19 +962,20 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -896,12 +1007,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>978455.0999839902</v>
+        <v>978455.09998399019</v>
       </c>
       <c r="C2">
         <v>51497.63684126264</v>
@@ -913,16 +1024,16 @@
         <v>1.918018601760066</v>
       </c>
       <c r="F2">
-        <v>0.07855448832375503</v>
+        <v>7.8554488323755028E-2</v>
       </c>
       <c r="G2">
-        <v>6162.060748991311</v>
+        <v>6162.0607489913109</v>
       </c>
       <c r="H2">
-        <v>78.49879457030733</v>
+        <v>78.498794570307325</v>
       </c>
       <c r="I2">
-        <v>5.976906786389425</v>
+        <v>5.9769067863894252</v>
       </c>
       <c r="J2" t="s">
         <v>30</v>
@@ -931,12 +1042,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>536987.8769059479</v>
+        <v>536987.87690594792</v>
       </c>
       <c r="C3">
         <v>26849.3938452974</v>
@@ -945,10 +1056,10 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>7.753341142689738</v>
+        <v>7.7533411426897381</v>
       </c>
       <c r="F3">
-        <v>2.461013124629633e-08</v>
+        <v>2.4610131246296332E-8</v>
       </c>
       <c r="G3">
         <v>11693.22442897335</v>
@@ -957,7 +1068,7 @@
         <v>108.1352136400227</v>
       </c>
       <c r="I3">
-        <v>8.233426969045384</v>
+        <v>8.2334269690453841</v>
       </c>
       <c r="J3" t="s">
         <v>31</v>
@@ -966,27 +1077,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>138517.7994940281</v>
+        <v>138517.79949402809</v>
       </c>
       <c r="C4">
-        <v>3462.944987350702</v>
+        <v>3462.9449873507019</v>
       </c>
       <c r="D4">
         <v>40</v>
       </c>
       <c r="G4">
-        <v>3462.944987350702</v>
+        <v>3462.9449873507019</v>
       </c>
       <c r="H4">
-        <v>58.84679249840812</v>
+        <v>58.846792498408121</v>
       </c>
       <c r="I4">
-        <v>4.480601203703412</v>
+        <v>4.4806012037034124</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -995,7 +1106,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1003,19 +1114,19 @@
         <v>1653960.776383966</v>
       </c>
       <c r="C5">
-        <v>20936.21235929071</v>
+        <v>20936.212359290708</v>
       </c>
       <c r="D5">
-        <v>41.1228820149699</v>
+        <v>41.122882014969903</v>
       </c>
       <c r="G5">
-        <v>21318.23016531536</v>
+        <v>21318.230165315359</v>
       </c>
       <c r="H5">
-        <v>146.0076373526925</v>
+        <v>146.00763735269251</v>
       </c>
       <c r="I5">
-        <v>11.11703744414043</v>
+        <v>11.117037444140429</v>
       </c>
       <c r="J5" t="s">
         <v>33</v>
@@ -1025,19 +1136,20 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,33 +1181,33 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>174917.6785076857</v>
+        <v>174917.67850768569</v>
       </c>
       <c r="C2">
-        <v>9206.193605667666</v>
+        <v>9206.1936056676659</v>
       </c>
       <c r="D2">
         <v>19</v>
       </c>
       <c r="E2">
-        <v>1.829882011789694</v>
+        <v>1.8298820117896939</v>
       </c>
       <c r="F2">
-        <v>0.09438266644156175</v>
+        <v>9.4382666441561749E-2</v>
       </c>
       <c r="G2">
         <v>1043.790586110609</v>
       </c>
       <c r="H2">
-        <v>32.30774808170029</v>
+        <v>32.307748081700289</v>
       </c>
       <c r="I2">
-        <v>5.682697307944562</v>
+        <v>5.6826973079445624</v>
       </c>
       <c r="J2" t="s">
         <v>38</v>
@@ -1104,12 +1216,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>100620.6252245046</v>
+        <v>100620.62522450461</v>
       </c>
       <c r="C3">
         <v>5031.031261225231</v>
@@ -1121,16 +1233,16 @@
         <v>5.922772914976985</v>
       </c>
       <c r="F3">
-        <v>9.390106226755859e-07</v>
+        <v>9.3901062267558588E-7</v>
       </c>
       <c r="G3">
-        <v>2090.796387325134</v>
+        <v>2090.7963873251342</v>
       </c>
       <c r="H3">
-        <v>45.72522703415626</v>
+        <v>45.725227034156262</v>
       </c>
       <c r="I3">
-        <v>8.04273401894369</v>
+        <v>8.0427340189436904</v>
       </c>
       <c r="J3" t="s">
         <v>39</v>
@@ -1139,27 +1251,27 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>33977.53946299851</v>
+        <v>33977.539462998509</v>
       </c>
       <c r="C4">
-        <v>849.4384865749628</v>
+        <v>849.43848657496278</v>
       </c>
       <c r="D4">
         <v>40</v>
       </c>
       <c r="G4">
-        <v>849.4384865749628</v>
+        <v>849.43848657496278</v>
       </c>
       <c r="H4">
         <v>29.14512800752405</v>
       </c>
       <c r="I4">
-        <v>5.126415497893166</v>
+        <v>5.1264154978931664</v>
       </c>
       <c r="J4" t="s">
         <v>40</v>
@@ -1168,24 +1280,24 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5">
-        <v>309515.8431951888</v>
+        <v>309515.84319518879</v>
       </c>
       <c r="C5">
         <v>3917.922065761883</v>
       </c>
       <c r="D5">
-        <v>43.79775849559376</v>
+        <v>43.797758495593762</v>
       </c>
       <c r="G5">
         <v>3984.025460010706</v>
       </c>
       <c r="H5">
-        <v>63.11913703474332</v>
+        <v>63.119137034743318</v>
       </c>
       <c r="I5">
         <v>11.10219595621667</v>
@@ -1198,6 +1310,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>